<commit_message>
new program + maeva abstract
</commit_message>
<xml_diff>
--- a/assets/forms/final_schedule.xlsx
+++ b/assets/forms/final_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphamanae/Documents/GitHub/honeybeehealth2021.github.io/assets/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2ECE76-0A61-8040-A6E0-31E146B470F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88E3742-8F0E-454A-B060-F4D15DE12AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{47551867-1369-F343-BD4D-B0AF0746D20B}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="5" xr2:uid="{47551867-1369-F343-BD4D-B0AF0746D20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="528">
   <si>
     <t>Monday 22 March</t>
   </si>
@@ -1334,24 +1334,9 @@
     <t>Fri 15:20</t>
   </si>
   <si>
-    <t>Fri 07:40</t>
-  </si>
-  <si>
-    <t>Fri 12:10</t>
-  </si>
-  <si>
-    <t>Fri 14:40</t>
-  </si>
-  <si>
-    <t>Fri 15:40</t>
-  </si>
-  <si>
     <t>Fri 08:00</t>
   </si>
   <si>
-    <t>Fri 15:00</t>
-  </si>
-  <si>
     <t>Fri 16:00</t>
   </si>
   <si>
@@ -1511,12 +1496,6 @@
     <t>Thu 23:20</t>
   </si>
   <si>
-    <t>Thu 23:40</t>
-  </si>
-  <si>
-    <t>Fri 00:00</t>
-  </si>
-  <si>
     <t>Fri 01:00</t>
   </si>
   <si>
@@ -1577,12 +1556,6 @@
     <t>Fri 17:20</t>
   </si>
   <si>
-    <t>Fri 17:40</t>
-  </si>
-  <si>
-    <t>Fri 18:00</t>
-  </si>
-  <si>
     <t>Fri 19:00</t>
   </si>
   <si>
@@ -1605,6 +1578,54 @@
   </si>
   <si>
     <t>Chuleui Jung</t>
+  </si>
+  <si>
+    <t>Vienna Kowallik</t>
+  </si>
+  <si>
+    <t>Fri 17:30</t>
+  </si>
+  <si>
+    <t>Fri 02:30</t>
+  </si>
+  <si>
+    <t>Thu 23:30</t>
+  </si>
+  <si>
+    <t>Fri 15:50</t>
+  </si>
+  <si>
+    <t>Fri 17:50</t>
+  </si>
+  <si>
+    <t>Fri 10:50</t>
+  </si>
+  <si>
+    <t>Fri 02:50</t>
+  </si>
+  <si>
+    <t>Thu 23:50</t>
+  </si>
+  <si>
+    <t>Fri 00:10</t>
+  </si>
+  <si>
+    <t>Fri 03:10</t>
+  </si>
+  <si>
+    <t>Fri 10:10</t>
+  </si>
+  <si>
+    <t>Fri 11:10</t>
+  </si>
+  <si>
+    <t>Fri 15:10</t>
+  </si>
+  <si>
+    <t>Fri 16:10</t>
+  </si>
+  <si>
+    <t>Fri 18:10</t>
   </si>
 </sst>
 </file>
@@ -2181,6 +2202,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2190,6 +2223,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2202,66 +2283,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2325,61 +2346,61 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2729,14 +2750,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -2757,10 +2778,10 @@
       <c r="F2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="70"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -2808,10 +2829,10 @@
       <c r="F5" s="10">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="I5" s="66" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2834,8 +2855,8 @@
       <c r="F6" s="10">
         <v>0.46527777777777773</v>
       </c>
-      <c r="H6" s="74"/>
-      <c r="I6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -2856,10 +2877,10 @@
       <c r="F7" s="10">
         <v>0.47222222222222227</v>
       </c>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="63"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -2880,8 +2901,8 @@
       <c r="F8" s="10">
         <v>0.47916666666666669</v>
       </c>
-      <c r="H8" s="76"/>
-      <c r="I8" s="61" t="s">
+      <c r="H8" s="64"/>
+      <c r="I8" s="66" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2904,8 +2925,8 @@
       <c r="F9" s="10">
         <v>0.4861111111111111</v>
       </c>
-      <c r="H9" s="76"/>
-      <c r="I9" s="62"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
@@ -2926,8 +2947,8 @@
       <c r="F10" s="10">
         <v>0.49305555555555558</v>
       </c>
-      <c r="H10" s="77"/>
-      <c r="I10" s="63"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="68"/>
     </row>
     <row r="11" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
@@ -2948,10 +2969,10 @@
       <c r="F11" s="10">
         <v>0.5</v>
       </c>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="61" t="s">
+      <c r="I11" s="66" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2974,8 +2995,8 @@
       <c r="F12" s="10">
         <v>0.50694444444444442</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
@@ -2996,8 +3017,8 @@
       <c r="F13" s="10">
         <v>0.51388888888888895</v>
       </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
     </row>
     <row r="14" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
@@ -3018,10 +3039,10 @@
       <c r="F14" s="10">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H14" s="64" t="s">
+      <c r="H14" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="69" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3044,8 +3065,8 @@
       <c r="F15" s="10">
         <v>0.52777777777777779</v>
       </c>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
     </row>
     <row r="16" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
@@ -3066,10 +3087,10 @@
       <c r="F16" s="10">
         <v>0.53472222222222221</v>
       </c>
-      <c r="H16" s="61" t="s">
+      <c r="H16" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="66" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3092,8 +3113,8 @@
       <c r="F17" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
     </row>
     <row r="18" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
@@ -3114,8 +3135,8 @@
       <c r="F18" s="10">
         <v>0.54861111111111105</v>
       </c>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
@@ -3136,10 +3157,10 @@
       <c r="F19" s="10">
         <v>0.55555555555555558</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="61" t="s">
+      <c r="I19" s="66" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3162,8 +3183,8 @@
       <c r="F20" s="10">
         <v>0.5625</v>
       </c>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
     </row>
     <row r="21" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
@@ -3184,8 +3205,8 @@
       <c r="F21" s="10">
         <v>0.56944444444444442</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
     </row>
     <row r="22" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
@@ -3254,10 +3275,10 @@
       <c r="F25" s="10">
         <v>0.64583333333333337</v>
       </c>
-      <c r="H25" s="61" t="s">
+      <c r="H25" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="54" t="s">
+      <c r="I25" s="58" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3280,8 +3301,8 @@
       <c r="F26" s="10">
         <v>0.65277777777777779</v>
       </c>
-      <c r="H26" s="62"/>
-      <c r="I26" s="55"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
@@ -3302,8 +3323,8 @@
       <c r="F27" s="10">
         <v>0.65972222222222221</v>
       </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="55"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
@@ -3324,10 +3345,10 @@
       <c r="F28" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H28" s="61" t="s">
+      <c r="H28" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I28" s="55"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
@@ -3348,8 +3369,8 @@
       <c r="F29" s="10">
         <v>0.67361111111111116</v>
       </c>
-      <c r="H29" s="62"/>
-      <c r="I29" s="55"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
@@ -3370,8 +3391,8 @@
       <c r="F30" s="10">
         <v>0.68055555555555547</v>
       </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="56"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="60"/>
     </row>
     <row r="31" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
@@ -3392,10 +3413,10 @@
       <c r="F31" s="10">
         <v>0.6875</v>
       </c>
-      <c r="H31" s="61" t="s">
+      <c r="H31" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I31" s="64" t="s">
+      <c r="I31" s="69" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3418,8 +3439,8 @@
       <c r="F32" s="10">
         <v>0.69444444444444453</v>
       </c>
-      <c r="H32" s="62"/>
-      <c r="I32" s="65"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="70"/>
     </row>
     <row r="33" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
@@ -3440,8 +3461,8 @@
       <c r="F33" s="10">
         <v>0.70138888888888884</v>
       </c>
-      <c r="H33" s="63"/>
-      <c r="I33" s="54" t="s">
+      <c r="H33" s="68"/>
+      <c r="I33" s="58" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3464,10 +3485,10 @@
       <c r="F34" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H34" s="64" t="s">
+      <c r="H34" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="55"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
@@ -3488,8 +3509,8 @@
       <c r="F35" s="10">
         <v>0.71527777777777779</v>
       </c>
-      <c r="H35" s="65"/>
-      <c r="I35" s="55"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
@@ -3510,10 +3531,10 @@
       <c r="F36" s="10">
         <v>0.72222222222222221</v>
       </c>
-      <c r="H36" s="61" t="s">
+      <c r="H36" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I36" s="55"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
@@ -3534,8 +3555,8 @@
       <c r="F37" s="10">
         <v>0.72916666666666663</v>
       </c>
-      <c r="H37" s="62"/>
-      <c r="I37" s="55"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
@@ -3556,8 +3577,8 @@
       <c r="F38" s="10">
         <v>0.73611111111111116</v>
       </c>
-      <c r="H38" s="63"/>
-      <c r="I38" s="55"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
@@ -3578,10 +3599,10 @@
       <c r="F39" s="10">
         <v>0.74305555555555547</v>
       </c>
-      <c r="H39" s="61" t="s">
+      <c r="H39" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="56"/>
+      <c r="I39" s="60"/>
     </row>
     <row r="40" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
@@ -3602,8 +3623,8 @@
       <c r="F40" s="10">
         <v>0.75</v>
       </c>
-      <c r="H40" s="62"/>
-      <c r="I40" s="78" t="s">
+      <c r="H40" s="67"/>
+      <c r="I40" s="71" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3626,8 +3647,8 @@
       <c r="F41" s="10">
         <v>0.75694444444444453</v>
       </c>
-      <c r="H41" s="63"/>
-      <c r="I41" s="79"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="72"/>
     </row>
     <row r="42" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
@@ -3649,7 +3670,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="H42" s="6"/>
-      <c r="I42" s="79"/>
+      <c r="I42" s="72"/>
     </row>
     <row r="43" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
@@ -3671,7 +3692,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="H43" s="6"/>
-      <c r="I43" s="79"/>
+      <c r="I43" s="72"/>
     </row>
     <row r="44" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
@@ -3693,7 +3714,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="H44" s="6"/>
-      <c r="I44" s="79"/>
+      <c r="I44" s="72"/>
     </row>
     <row r="45" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
@@ -3715,7 +3736,7 @@
         <v>0.8125</v>
       </c>
       <c r="H45" s="6"/>
-      <c r="I45" s="80"/>
+      <c r="I45" s="73"/>
     </row>
     <row r="46" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
@@ -3736,14 +3757,14 @@
       <c r="K47" s="6"/>
     </row>
     <row r="48" spans="1:11" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="60" t="s">
+      <c r="A48" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="60"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
     </row>
     <row r="49" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -3764,11 +3785,11 @@
       <c r="F49" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="57" t="s">
+      <c r="H49" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="I49" s="58"/>
-      <c r="J49" s="59"/>
+      <c r="I49" s="78"/>
+      <c r="J49" s="79"/>
     </row>
     <row r="50" spans="1:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
@@ -3831,13 +3852,13 @@
       <c r="F52" s="10">
         <v>0.85416666666666663</v>
       </c>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I52" s="54" t="s">
+      <c r="I52" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="J52" s="54" t="s">
+      <c r="J52" s="58" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3860,9 +3881,9 @@
       <c r="F53" s="10">
         <v>0.86111111111111116</v>
       </c>
-      <c r="H53" s="72"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
     </row>
     <row r="54" spans="1:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
@@ -3883,11 +3904,11 @@
       <c r="F54" s="10">
         <v>0.86805555555555547</v>
       </c>
-      <c r="H54" s="54" t="s">
+      <c r="H54" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="I54" s="56"/>
-      <c r="J54" s="56"/>
+      <c r="I54" s="60"/>
+      <c r="J54" s="60"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
     </row>
@@ -3910,11 +3931,11 @@
       <c r="F55" s="10">
         <v>0.875</v>
       </c>
-      <c r="H55" s="55"/>
-      <c r="I55" s="54" t="s">
+      <c r="H55" s="59"/>
+      <c r="I55" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J55" s="54" t="s">
+      <c r="J55" s="58" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3937,9 +3958,9 @@
       <c r="F56" s="10">
         <v>0.88194444444444453</v>
       </c>
-      <c r="H56" s="56"/>
-      <c r="I56" s="55"/>
-      <c r="J56" s="55"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="59"/>
     </row>
     <row r="57" spans="1:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
@@ -3960,11 +3981,11 @@
       <c r="F57" s="10">
         <v>0.88888888888888884</v>
       </c>
-      <c r="H57" s="54" t="s">
+      <c r="H57" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="I57" s="56"/>
-      <c r="J57" s="56"/>
+      <c r="I57" s="60"/>
+      <c r="J57" s="60"/>
     </row>
     <row r="58" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="10">
@@ -3985,11 +4006,11 @@
       <c r="F58" s="10">
         <v>0.89583333333333337</v>
       </c>
-      <c r="H58" s="55"/>
-      <c r="I58" s="54" t="s">
+      <c r="H58" s="59"/>
+      <c r="I58" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="J58" s="54" t="s">
+      <c r="J58" s="58" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4012,9 +4033,9 @@
       <c r="F59" s="10">
         <v>0.90277777777777779</v>
       </c>
-      <c r="H59" s="56"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
     </row>
     <row r="60" spans="1:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
@@ -4035,11 +4056,11 @@
       <c r="F60" s="10">
         <v>0.90972222222222221</v>
       </c>
-      <c r="H60" s="64" t="s">
+      <c r="H60" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="60"/>
       <c r="K60" s="6"/>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
@@ -4064,11 +4085,11 @@
       <c r="F61" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="H61" s="65"/>
-      <c r="I61" s="64" t="s">
+      <c r="H61" s="70"/>
+      <c r="I61" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="J61" s="64" t="s">
+      <c r="J61" s="69" t="s">
         <v>25</v>
       </c>
       <c r="K61" s="6"/>
@@ -4095,11 +4116,11 @@
       <c r="F62" s="10">
         <v>0.92361111111111116</v>
       </c>
-      <c r="H62" s="54" t="s">
+      <c r="H62" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I62" s="65"/>
-      <c r="J62" s="65"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
       <c r="K62" s="6"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
@@ -4123,11 +4144,11 @@
       <c r="F63" s="10">
         <v>0.93055555555555547</v>
       </c>
-      <c r="H63" s="55"/>
-      <c r="I63" s="54" t="s">
+      <c r="H63" s="59"/>
+      <c r="I63" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="J63" s="54" t="s">
+      <c r="J63" s="58" t="s">
         <v>24</v>
       </c>
       <c r="K63" s="6"/>
@@ -4153,9 +4174,9 @@
       <c r="F64" s="10">
         <v>0.9375</v>
       </c>
-      <c r="H64" s="56"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="55"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="59"/>
+      <c r="J64" s="59"/>
       <c r="K64" s="6"/>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
@@ -4179,11 +4200,11 @@
       <c r="F65" s="10">
         <v>0.94444444444444453</v>
       </c>
-      <c r="H65" s="54" t="s">
+      <c r="H65" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
+      <c r="I65" s="60"/>
+      <c r="J65" s="60"/>
       <c r="K65" s="6"/>
       <c r="L65" s="1"/>
       <c r="M65" s="6"/>
@@ -4208,11 +4229,11 @@
       <c r="F66" s="10">
         <v>0.95138888888888884</v>
       </c>
-      <c r="H66" s="55"/>
-      <c r="I66" s="54" t="s">
+      <c r="H66" s="59"/>
+      <c r="I66" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="J66" s="66" t="s">
+      <c r="J66" s="74" t="s">
         <v>42</v>
       </c>
       <c r="K66" s="6"/>
@@ -4239,9 +4260,9 @@
       <c r="F67" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="H67" s="56"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="67"/>
+      <c r="H67" s="60"/>
+      <c r="I67" s="59"/>
+      <c r="J67" s="75"/>
       <c r="K67" s="6"/>
       <c r="L67" s="3"/>
       <c r="M67" s="6"/>
@@ -4266,11 +4287,11 @@
       <c r="F68" s="10">
         <v>0.96527777777777779</v>
       </c>
-      <c r="H68" s="64" t="s">
+      <c r="H68" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="I68" s="56"/>
-      <c r="J68" s="67"/>
+      <c r="I68" s="60"/>
+      <c r="J68" s="75"/>
       <c r="K68" s="6"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -4295,11 +4316,11 @@
       <c r="F69" s="10">
         <v>0.97222222222222221</v>
       </c>
-      <c r="H69" s="65"/>
-      <c r="I69" s="66" t="s">
+      <c r="H69" s="70"/>
+      <c r="I69" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="J69" s="68"/>
+      <c r="J69" s="76"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
@@ -4324,10 +4345,10 @@
       <c r="F70" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="H70" s="54" t="s">
+      <c r="H70" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="I70" s="67"/>
+      <c r="I70" s="75"/>
       <c r="J70" s="11" t="s">
         <v>32</v>
       </c>
@@ -4355,8 +4376,8 @@
       <c r="F71" s="10">
         <v>0.98611111111111116</v>
       </c>
-      <c r="H71" s="55"/>
-      <c r="I71" s="67"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="75"/>
       <c r="J71" s="12"/>
       <c r="K71" s="6"/>
       <c r="L71" s="3"/>
@@ -4382,8 +4403,8 @@
       <c r="F72" s="10">
         <v>0.99305555555555547</v>
       </c>
-      <c r="H72" s="56"/>
-      <c r="I72" s="68"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="76"/>
       <c r="J72" s="12"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
@@ -4510,21 +4531,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="H54:H56"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="I25:I30"/>
-    <mergeCell ref="I40:I45"/>
+    <mergeCell ref="J58:J60"/>
+    <mergeCell ref="H70:H72"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="I33:I39"/>
     <mergeCell ref="H60:H61"/>
     <mergeCell ref="H62:H64"/>
     <mergeCell ref="H65:H67"/>
@@ -4541,22 +4563,21 @@
     <mergeCell ref="I69:I72"/>
     <mergeCell ref="J63:J65"/>
     <mergeCell ref="J61:J62"/>
-    <mergeCell ref="J58:J60"/>
-    <mergeCell ref="H70:H72"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="I33:I39"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="I40:I45"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="85" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4721,11 +4742,11 @@
       <c r="J4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="K4" s="71" t="s">
+      <c r="K4" s="56" t="s">
         <v>149</v>
       </c>
       <c r="L4" s="83" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="M4" s="34"/>
     </row>
@@ -4758,7 +4779,7 @@
       <c r="J5" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="K5" s="72"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="84"/>
       <c r="M5" s="34"/>
     </row>
@@ -5582,7 +5603,7 @@
         <v>154</v>
       </c>
       <c r="L4" s="83" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="M4" s="34"/>
     </row>
@@ -6439,7 +6460,7 @@
         <v>222</v>
       </c>
       <c r="L4" s="95" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="M4" s="34"/>
     </row>
@@ -6767,7 +6788,7 @@
         <v>268</v>
       </c>
       <c r="K16" s="96" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="L16" s="95"/>
       <c r="M16" s="34"/>
@@ -6860,7 +6881,7 @@
         <v>230</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>233</v>
@@ -6881,7 +6902,7 @@
         <v>253</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="K20" s="101"/>
       <c r="L20" s="95"/>
@@ -6907,7 +6928,7 @@
         <v>230</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>233</v>
@@ -6928,7 +6949,7 @@
         <v>253</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="K22" s="52" t="s">
         <v>32</v>
@@ -7023,7 +7044,7 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N51" sqref="A1:N51"/>
     </sheetView>
   </sheetViews>
@@ -7071,10 +7092,10 @@
       <c r="J1" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="106" t="s">
+      <c r="K1" s="104" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="107"/>
+      <c r="L1" s="105"/>
       <c r="M1" s="34"/>
       <c r="N1" s="34"/>
     </row>
@@ -7109,8 +7130,8 @@
       <c r="J2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="107"/>
       <c r="M2" s="34"/>
       <c r="N2" s="34"/>
     </row>
@@ -7145,18 +7166,18 @@
       <c r="J3" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="110"/>
-      <c r="L3" s="111"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="109"/>
       <c r="M3" s="34"/>
       <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="27" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>282</v>
@@ -7179,12 +7200,12 @@
       <c r="J4" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="K4" s="112" t="s">
+      <c r="K4" s="110" t="s">
         <v>348</v>
       </c>
       <c r="L4" s="37"/>
       <c r="M4" s="83" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="N4" s="34"/>
     </row>
@@ -7217,7 +7238,7 @@
       <c r="J5" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="K5" s="113"/>
+      <c r="K5" s="111"/>
       <c r="L5" s="37"/>
       <c r="M5" s="84"/>
       <c r="N5" s="34"/>
@@ -7267,7 +7288,7 @@
       <c r="J7" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="K7" s="112" t="s">
+      <c r="K7" s="110" t="s">
         <v>349</v>
       </c>
       <c r="L7" s="37"/>
@@ -7303,7 +7324,7 @@
       <c r="J8" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="K8" s="113"/>
+      <c r="K8" s="111"/>
       <c r="L8" s="37"/>
       <c r="M8" s="84"/>
       <c r="N8" s="53"/>
@@ -7353,7 +7374,7 @@
       <c r="J10" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="K10" s="104" t="s">
+      <c r="K10" s="102" t="s">
         <v>350</v>
       </c>
       <c r="L10" s="37"/>
@@ -7364,10 +7385,10 @@
     <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="27" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>300</v>
@@ -7390,7 +7411,7 @@
       <c r="J11" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="K11" s="105"/>
+      <c r="K11" s="103"/>
       <c r="L11" s="37"/>
       <c r="M11" s="84"/>
       <c r="N11" s="53"/>
@@ -7414,10 +7435,10 @@
     <row r="13" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
       <c r="B13" s="27" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>300</v>
@@ -7440,7 +7461,7 @@
       <c r="J13" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="K13" s="104" t="s">
+      <c r="K13" s="102" t="s">
         <v>351</v>
       </c>
       <c r="L13" s="37"/>
@@ -7450,10 +7471,10 @@
     <row r="14" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="27" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>306</v>
@@ -7476,7 +7497,7 @@
       <c r="J14" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="K14" s="105"/>
+      <c r="K14" s="103"/>
       <c r="L14" s="37"/>
       <c r="M14" s="84"/>
       <c r="N14" s="34"/>
@@ -7500,10 +7521,10 @@
     <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37"/>
       <c r="B16" s="27" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D16" s="27" t="s">
         <v>306</v>
@@ -7526,7 +7547,7 @@
       <c r="J16" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="K16" s="104" t="s">
+      <c r="K16" s="102" t="s">
         <v>353</v>
       </c>
       <c r="L16" s="37"/>
@@ -7539,7 +7560,7 @@
         <v>252</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D17" s="27" t="s">
         <v>295</v>
@@ -7562,7 +7583,7 @@
       <c r="J17" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="K17" s="105"/>
+      <c r="K17" s="103"/>
       <c r="L17" s="37"/>
       <c r="M17" s="84"/>
       <c r="N17" s="34"/>
@@ -7589,7 +7610,7 @@
         <v>252</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>295</v>
@@ -7612,7 +7633,7 @@
       <c r="J19" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="K19" s="104" t="s">
+      <c r="K19" s="102" t="s">
         <v>352</v>
       </c>
       <c r="L19" s="37"/>
@@ -7646,9 +7667,9 @@
         <v>317</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="K20" s="105"/>
+        <v>465</v>
+      </c>
+      <c r="K20" s="103"/>
       <c r="L20" s="37"/>
       <c r="M20" s="84"/>
       <c r="N20" s="34"/>
@@ -7696,9 +7717,9 @@
         <v>317</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="K22" s="104" t="s">
+        <v>465</v>
+      </c>
+      <c r="K22" s="102" t="s">
         <v>354</v>
       </c>
       <c r="L22" s="37"/>
@@ -7708,10 +7729,10 @@
     <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="27" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D23" s="27" t="s">
         <v>307</v>
@@ -7732,9 +7753,9 @@
         <v>320</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>471</v>
-      </c>
-      <c r="K23" s="105"/>
+        <v>466</v>
+      </c>
+      <c r="K23" s="103"/>
       <c r="L23" s="37"/>
       <c r="M23" s="84"/>
       <c r="N23" s="34"/>
@@ -7761,7 +7782,7 @@
         <v>259</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>321</v>
@@ -7784,10 +7805,10 @@
       <c r="J25" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="K25" s="104" t="s">
+      <c r="K25" s="102" t="s">
         <v>355</v>
       </c>
-      <c r="L25" s="102" t="s">
+      <c r="L25" s="112" t="s">
         <v>361</v>
       </c>
       <c r="M25" s="84"/>
@@ -7799,7 +7820,7 @@
         <v>268</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>324</v>
@@ -7822,8 +7843,8 @@
       <c r="J26" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="K26" s="105"/>
-      <c r="L26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="113"/>
       <c r="M26" s="84"/>
       <c r="N26" s="34"/>
     </row>
@@ -7849,7 +7870,7 @@
         <v>268</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>324</v>
@@ -7872,10 +7893,10 @@
       <c r="J28" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="K28" s="104" t="s">
+      <c r="K28" s="102" t="s">
         <v>356</v>
       </c>
-      <c r="L28" s="102" t="s">
+      <c r="L28" s="112" t="s">
         <v>362</v>
       </c>
       <c r="M28" s="84"/>
@@ -7884,7 +7905,7 @@
     <row r="29" spans="1:14" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="27" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>282</v>
@@ -7910,8 +7931,8 @@
       <c r="J29" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="K29" s="105"/>
-      <c r="L29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="113"/>
       <c r="M29" s="84"/>
       <c r="N29" s="34"/>
     </row>
@@ -7934,7 +7955,7 @@
     <row r="31" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="27" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>282</v>
@@ -7960,10 +7981,10 @@
       <c r="J31" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="K31" s="104" t="s">
-        <v>514</v>
-      </c>
-      <c r="L31" s="102" t="s">
+      <c r="K31" s="102" t="s">
+        <v>505</v>
+      </c>
+      <c r="L31" s="112" t="s">
         <v>363</v>
       </c>
       <c r="M31" s="84"/>
@@ -7972,7 +7993,7 @@
     <row r="32" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" s="27" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>288</v>
@@ -7998,8 +8019,8 @@
       <c r="J32" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="K32" s="105"/>
-      <c r="L32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="113"/>
       <c r="M32" s="84"/>
       <c r="N32" s="34"/>
     </row>
@@ -8022,7 +8043,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="37"/>
       <c r="B34" s="27" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>288</v>
@@ -8048,10 +8069,10 @@
       <c r="J34" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="K34" s="104" t="s">
-        <v>520</v>
-      </c>
-      <c r="L34" s="102" t="s">
+      <c r="K34" s="102" t="s">
+        <v>511</v>
+      </c>
+      <c r="L34" s="112" t="s">
         <v>364</v>
       </c>
       <c r="M34" s="84"/>
@@ -8063,7 +8084,7 @@
         <v>278</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D35" s="27" t="s">
         <v>303</v>
@@ -8084,10 +8105,10 @@
         <v>333</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="K35" s="105"/>
-      <c r="L35" s="103"/>
+        <v>467</v>
+      </c>
+      <c r="K35" s="103"/>
+      <c r="L35" s="113"/>
       <c r="M35" s="84"/>
       <c r="N35" s="34"/>
     </row>
@@ -8113,7 +8134,7 @@
         <v>278</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D37" s="27" t="s">
         <v>303</v>
@@ -8134,7 +8155,7 @@
         <v>333</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="K37" s="91" t="s">
         <v>25</v>
@@ -8148,7 +8169,7 @@
     <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37"/>
       <c r="B38" s="27" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>283</v>
@@ -8172,7 +8193,7 @@
         <v>335</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="K38" s="92"/>
       <c r="L38" s="99"/>
@@ -8198,7 +8219,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="37"/>
       <c r="B40" s="27" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>283</v>
@@ -8222,12 +8243,12 @@
         <v>335</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>473</v>
-      </c>
-      <c r="K40" s="104" t="s">
+        <v>468</v>
+      </c>
+      <c r="K40" s="102" t="s">
         <v>357</v>
       </c>
-      <c r="L40" s="102" t="s">
+      <c r="L40" s="112" t="s">
         <v>365</v>
       </c>
       <c r="M40" s="84"/>
@@ -8260,10 +8281,10 @@
         <v>338</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>474</v>
-      </c>
-      <c r="K41" s="105"/>
-      <c r="L41" s="103"/>
+        <v>469</v>
+      </c>
+      <c r="K41" s="103"/>
+      <c r="L41" s="113"/>
       <c r="M41" s="84"/>
       <c r="N41" s="34"/>
     </row>
@@ -8310,12 +8331,12 @@
         <v>338</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>474</v>
-      </c>
-      <c r="K43" s="104" t="s">
+        <v>469</v>
+      </c>
+      <c r="K43" s="102" t="s">
         <v>358</v>
       </c>
-      <c r="L43" s="102" t="s">
+      <c r="L43" s="112" t="s">
         <v>366</v>
       </c>
       <c r="M43" s="84"/>
@@ -8324,10 +8345,10 @@
     <row r="44" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
       <c r="B44" s="27" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D44" s="27" t="s">
         <v>316</v>
@@ -8348,10 +8369,10 @@
         <v>341</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>475</v>
-      </c>
-      <c r="K44" s="105"/>
-      <c r="L44" s="103"/>
+        <v>470</v>
+      </c>
+      <c r="K44" s="103"/>
+      <c r="L44" s="113"/>
       <c r="M44" s="84"/>
       <c r="N44" s="34"/>
     </row>
@@ -8374,10 +8395,10 @@
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="27"/>
       <c r="B46" s="27" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D46" s="27" t="s">
         <v>316</v>
@@ -8398,12 +8419,12 @@
         <v>341</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>475</v>
-      </c>
-      <c r="K46" s="104" t="s">
+        <v>470</v>
+      </c>
+      <c r="K46" s="102" t="s">
         <v>359</v>
       </c>
-      <c r="L46" s="102" t="s">
+      <c r="L46" s="112" t="s">
         <v>367</v>
       </c>
       <c r="M46" s="84"/>
@@ -8412,10 +8433,10 @@
     <row r="47" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
       <c r="B47" s="27" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D47" s="27" t="s">
         <v>286</v>
@@ -8436,10 +8457,10 @@
         <v>344</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>476</v>
-      </c>
-      <c r="K47" s="105"/>
-      <c r="L47" s="103"/>
+        <v>471</v>
+      </c>
+      <c r="K47" s="103"/>
+      <c r="L47" s="113"/>
       <c r="M47" s="84"/>
       <c r="N47" s="34"/>
     </row>
@@ -8462,10 +8483,10 @@
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="27"/>
       <c r="B49" s="27" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D49" s="27" t="s">
         <v>286</v>
@@ -8486,12 +8507,12 @@
         <v>344</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>476</v>
-      </c>
-      <c r="K49" s="104" t="s">
+        <v>471</v>
+      </c>
+      <c r="K49" s="102" t="s">
         <v>360</v>
       </c>
-      <c r="L49" s="102" t="s">
+      <c r="L49" s="112" t="s">
         <v>368</v>
       </c>
       <c r="M49" s="84"/>
@@ -8500,10 +8521,10 @@
     <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27"/>
       <c r="B50" s="27" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D50" s="27" t="s">
         <v>292</v>
@@ -8524,10 +8545,10 @@
         <v>347</v>
       </c>
       <c r="J50" s="27" t="s">
-        <v>477</v>
-      </c>
-      <c r="K50" s="105"/>
-      <c r="L50" s="103"/>
+        <v>472</v>
+      </c>
+      <c r="K50" s="103"/>
+      <c r="L50" s="113"/>
       <c r="M50" s="85"/>
       <c r="N50" s="34"/>
     </row>
@@ -8565,17 +8586,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="K1:L3"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="K25:K26"/>
     <mergeCell ref="L49:L50"/>
     <mergeCell ref="M4:M50"/>
     <mergeCell ref="K46:K47"/>
@@ -8592,6 +8602,17 @@
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="K34:K35"/>
     <mergeCell ref="K37:K38"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="K1:L3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K25:K26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="93" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -8603,10 +8624,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M54" sqref="B1:M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8653,7 +8674,7 @@
       <c r="J1" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="K1" s="114" t="s">
         <v>369</v>
       </c>
       <c r="L1" s="34"/>
@@ -8689,7 +8710,7 @@
       <c r="J2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="117"/>
+      <c r="K2" s="115"/>
       <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -8723,23 +8744,23 @@
       <c r="J3" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="118"/>
+      <c r="K3" s="116"/>
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="27" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>372</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>373</v>
@@ -8756,21 +8777,21 @@
       <c r="J4" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="K4" s="119" t="s">
+      <c r="K4" s="117" t="s">
         <v>348</v>
       </c>
       <c r="L4" s="83" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="27" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>377</v>
@@ -8793,7 +8814,7 @@
       <c r="J5" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="K5" s="120"/>
+      <c r="K5" s="118"/>
       <c r="L5" s="84"/>
       <c r="M5" s="34"/>
     </row>
@@ -8815,10 +8836,10 @@
     <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="37"/>
       <c r="B7" s="27" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>377</v>
@@ -8841,8 +8862,8 @@
       <c r="J7" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="K7" s="102" t="s">
-        <v>438</v>
+      <c r="K7" s="112" t="s">
+        <v>433</v>
       </c>
       <c r="L7" s="84"/>
       <c r="M7" s="34"/>
@@ -8850,10 +8871,10 @@
     <row r="8" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="27" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>382</v>
@@ -8876,7 +8897,7 @@
       <c r="J8" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="K8" s="103"/>
+      <c r="K8" s="113"/>
       <c r="L8" s="84"/>
       <c r="M8" s="34"/>
     </row>
@@ -8898,10 +8919,10 @@
     <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="27" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>382</v>
@@ -8924,8 +8945,8 @@
       <c r="J10" s="27" t="s">
         <v>409</v>
       </c>
-      <c r="K10" s="102" t="s">
-        <v>439</v>
+      <c r="K10" s="112" t="s">
+        <v>434</v>
       </c>
       <c r="L10" s="84"/>
       <c r="M10" s="34"/>
@@ -8933,16 +8954,16 @@
     <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="27" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>387</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>388</v>
@@ -8959,7 +8980,7 @@
       <c r="J11" s="27" t="s">
         <v>413</v>
       </c>
-      <c r="K11" s="103"/>
+      <c r="K11" s="113"/>
       <c r="L11" s="84"/>
       <c r="M11" s="34"/>
     </row>
@@ -8981,16 +9002,16 @@
     <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
       <c r="B13" s="27" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>387</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>388</v>
@@ -9007,8 +9028,8 @@
       <c r="J13" s="27" t="s">
         <v>413</v>
       </c>
-      <c r="K13" s="102" t="s">
-        <v>440</v>
+      <c r="K13" s="112" t="s">
+        <v>435</v>
       </c>
       <c r="L13" s="84"/>
       <c r="M13" s="34"/>
@@ -9016,10 +9037,10 @@
     <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="27" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>392</v>
@@ -9042,7 +9063,7 @@
       <c r="J14" s="27" t="s">
         <v>421</v>
       </c>
-      <c r="K14" s="103"/>
+      <c r="K14" s="113"/>
       <c r="L14" s="84"/>
       <c r="M14" s="34"/>
     </row>
@@ -9064,10 +9085,10 @@
     <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37"/>
       <c r="B16" s="27" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D16" s="27" t="s">
         <v>392</v>
@@ -9099,10 +9120,10 @@
     <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="27" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D17" s="27" t="s">
         <v>396</v>
@@ -9123,7 +9144,7 @@
         <v>398</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="K17" s="99"/>
       <c r="L17" s="84"/>
@@ -9147,10 +9168,10 @@
     <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="27" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>396</v>
@@ -9171,10 +9192,10 @@
         <v>398</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="K19" s="102" t="s">
-        <v>441</v>
+        <v>498</v>
+      </c>
+      <c r="K19" s="112" t="s">
+        <v>436</v>
       </c>
       <c r="L19" s="84"/>
       <c r="M19" s="34"/>
@@ -9182,10 +9203,10 @@
     <row r="20" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37"/>
       <c r="B20" s="27" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>399</v>
@@ -9208,7 +9229,7 @@
       <c r="J20" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="K20" s="103"/>
+      <c r="K20" s="113"/>
       <c r="L20" s="84"/>
       <c r="M20" s="34"/>
     </row>
@@ -9230,10 +9251,10 @@
     <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="27" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>399</v>
@@ -9256,8 +9277,8 @@
       <c r="J22" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="K22" s="102" t="s">
-        <v>442</v>
+      <c r="K22" s="112" t="s">
+        <v>437</v>
       </c>
       <c r="L22" s="84"/>
       <c r="M22" s="34"/>
@@ -9265,10 +9286,10 @@
     <row r="23" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="27" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D23" s="27" t="s">
         <v>403</v>
@@ -9291,7 +9312,7 @@
       <c r="J23" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="K23" s="103"/>
+      <c r="K23" s="113"/>
       <c r="L23" s="84"/>
       <c r="M23" s="34"/>
     </row>
@@ -9313,10 +9334,10 @@
     <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="27" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>403</v>
@@ -9339,8 +9360,8 @@
       <c r="J25" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="K25" s="102" t="s">
-        <v>443</v>
+      <c r="K25" s="112" t="s">
+        <v>438</v>
       </c>
       <c r="L25" s="84"/>
       <c r="M25" s="34"/>
@@ -9348,10 +9369,10 @@
     <row r="26" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" s="27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>407</v>
@@ -9374,7 +9395,7 @@
       <c r="J26" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="K26" s="103"/>
+      <c r="K26" s="113"/>
       <c r="L26" s="85"/>
       <c r="M26" s="34"/>
     </row>
@@ -9396,10 +9417,10 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="37"/>
       <c r="B28" s="27" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>410</v>
@@ -9420,29 +9441,29 @@
         <v>412</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="K28" s="114" t="s">
-        <v>516</v>
+        <v>499</v>
+      </c>
+      <c r="K28" s="119" t="s">
+        <v>507</v>
       </c>
       <c r="L28" s="83" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="M28" s="34"/>
     </row>
     <row r="29" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="27" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="D29" s="27" t="s">
         <v>415</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="F29" s="27" t="s">
         <v>416</v>
@@ -9457,9 +9478,9 @@
         <v>419</v>
       </c>
       <c r="J29" s="27" t="s">
-        <v>507</v>
-      </c>
-      <c r="K29" s="115"/>
+        <v>500</v>
+      </c>
+      <c r="K29" s="120"/>
       <c r="L29" s="84"/>
       <c r="M29" s="34"/>
     </row>
@@ -9481,16 +9502,16 @@
     <row r="31" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="27" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>415</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="F31" s="27" t="s">
         <v>416</v>
@@ -9505,10 +9526,10 @@
         <v>419</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>507</v>
-      </c>
-      <c r="K31" s="114" t="s">
-        <v>517</v>
+        <v>500</v>
+      </c>
+      <c r="K31" s="119" t="s">
+        <v>508</v>
       </c>
       <c r="L31" s="84"/>
       <c r="M31" s="34"/>
@@ -9516,16 +9537,16 @@
     <row r="32" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" s="27" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D32" s="27" t="s">
         <v>393</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F32" s="27" t="s">
         <v>380</v>
@@ -9540,9 +9561,9 @@
         <v>422</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>436</v>
-      </c>
-      <c r="K32" s="115"/>
+        <v>431</v>
+      </c>
+      <c r="K32" s="120"/>
       <c r="L32" s="84"/>
       <c r="M32" s="34"/>
     </row>
@@ -9564,16 +9585,16 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="37"/>
       <c r="B34" s="27" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D34" s="27" t="s">
         <v>393</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F34" s="27" t="s">
         <v>380</v>
@@ -9588,9 +9609,9 @@
         <v>422</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>436</v>
-      </c>
-      <c r="K34" s="114" t="s">
+        <v>431</v>
+      </c>
+      <c r="K34" s="119" t="s">
         <v>146</v>
       </c>
       <c r="L34" s="84"/>
@@ -9599,10 +9620,10 @@
     <row r="35" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37"/>
       <c r="B35" s="27" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="D35" s="27" t="s">
         <v>379</v>
@@ -9623,9 +9644,9 @@
         <v>424</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>508</v>
-      </c>
-      <c r="K35" s="115"/>
+        <v>501</v>
+      </c>
+      <c r="K35" s="120"/>
       <c r="L35" s="84"/>
       <c r="M35" s="34"/>
     </row>
@@ -9647,10 +9668,10 @@
     <row r="37" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="37"/>
       <c r="B37" s="27" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="D37" s="27" t="s">
         <v>379</v>
@@ -9671,7 +9692,7 @@
         <v>424</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="K37" s="98" t="s">
         <v>25</v>
@@ -9682,7 +9703,7 @@
     <row r="38" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37"/>
       <c r="B38" s="27" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>372</v>
@@ -9706,7 +9727,7 @@
         <v>426</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="K38" s="99"/>
       <c r="L38" s="84"/>
@@ -9730,7 +9751,7 @@
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="37"/>
       <c r="B40" s="27" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>372</v>
@@ -9754,10 +9775,10 @@
         <v>426</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>509</v>
-      </c>
-      <c r="K40" s="114" t="s">
-        <v>444</v>
+        <v>502</v>
+      </c>
+      <c r="K40" s="119" t="s">
+        <v>439</v>
       </c>
       <c r="L40" s="84"/>
       <c r="M40" s="34"/>
@@ -9765,7 +9786,7 @@
     <row r="41" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37"/>
       <c r="B41" s="27" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>382</v>
@@ -9789,9 +9810,9 @@
         <v>429</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>510</v>
-      </c>
-      <c r="K41" s="115"/>
+        <v>503</v>
+      </c>
+      <c r="K41" s="120"/>
       <c r="L41" s="84"/>
       <c r="M41" s="34"/>
     </row>
@@ -9813,7 +9834,7 @@
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="27"/>
       <c r="B43" s="27" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>382</v>
@@ -9837,10 +9858,10 @@
         <v>429</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>510</v>
-      </c>
-      <c r="K43" s="114" t="s">
-        <v>353</v>
+        <v>503</v>
+      </c>
+      <c r="K43" s="119" t="s">
+        <v>512</v>
       </c>
       <c r="L43" s="84"/>
       <c r="M43" s="34"/>
@@ -9848,33 +9869,33 @@
     <row r="44" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
       <c r="B44" s="27" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>387</v>
+        <v>514</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>390</v>
+        <v>423</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>431</v>
+        <v>406</v>
       </c>
       <c r="H44" s="27" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="I44" s="26" t="s">
-        <v>433</v>
+        <v>499</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>511</v>
-      </c>
-      <c r="K44" s="115"/>
+        <v>513</v>
+      </c>
+      <c r="K44" s="120"/>
       <c r="L44" s="84"/>
       <c r="M44" s="34"/>
     </row>
@@ -9896,34 +9917,34 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="27"/>
       <c r="B46" s="27" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>387</v>
+        <v>514</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>390</v>
+        <v>423</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>431</v>
+        <v>406</v>
       </c>
       <c r="H46" s="27" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="I46" s="26" t="s">
-        <v>433</v>
+        <v>499</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>511</v>
-      </c>
-      <c r="K46" s="114" t="s">
-        <v>445</v>
+        <v>513</v>
+      </c>
+      <c r="K46" s="119" t="s">
+        <v>353</v>
       </c>
       <c r="L46" s="84"/>
       <c r="M46" s="34"/>
@@ -9931,33 +9952,33 @@
     <row r="47" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
       <c r="B47" s="27" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>392</v>
+        <v>519</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>434</v>
+        <v>397</v>
       </c>
       <c r="E47" s="27" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F47" s="27" t="s">
-        <v>395</v>
+        <v>518</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H47" s="27" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="I47" s="26" t="s">
-        <v>436</v>
+        <v>516</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>512</v>
-      </c>
-      <c r="K47" s="115"/>
+        <v>517</v>
+      </c>
+      <c r="K47" s="120"/>
       <c r="L47" s="84"/>
       <c r="M47" s="34"/>
     </row>
@@ -9972,41 +9993,41 @@
       <c r="H48" s="27"/>
       <c r="I48" s="26"/>
       <c r="J48" s="27"/>
-      <c r="K48" s="37"/>
+      <c r="K48" s="34"/>
       <c r="L48" s="84"/>
       <c r="M48" s="34"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="27"/>
       <c r="B49" s="27" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>392</v>
+        <v>519</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>434</v>
+        <v>397</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F49" s="27" t="s">
-        <v>395</v>
+        <v>518</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>436</v>
+        <v>516</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>512</v>
-      </c>
-      <c r="K49" s="100" t="s">
-        <v>446</v>
+        <v>517</v>
+      </c>
+      <c r="K49" s="119" t="s">
+        <v>440</v>
       </c>
       <c r="L49" s="84"/>
       <c r="M49" s="34"/>
@@ -10014,79 +10035,157 @@
     <row r="50" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27"/>
       <c r="B50" s="27" t="s">
-        <v>491</v>
+        <v>521</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>403</v>
+        <v>522</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>395</v>
+        <v>523</v>
       </c>
       <c r="F50" s="27" t="s">
-        <v>406</v>
+        <v>524</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>436</v>
+        <v>525</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>437</v>
+        <v>526</v>
       </c>
       <c r="J50" s="27" t="s">
-        <v>513</v>
-      </c>
-      <c r="K50" s="101"/>
-      <c r="L50" s="85"/>
+        <v>527</v>
+      </c>
+      <c r="K50" s="120"/>
+      <c r="L50" s="84"/>
       <c r="M50" s="34"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="84"/>
       <c r="M51" s="34"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="27"/>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
+      <c r="B52" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>522</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>523</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>524</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="H52" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="I52" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="J52" s="27" t="s">
+        <v>527</v>
+      </c>
+      <c r="K52" s="100" t="s">
+        <v>441</v>
+      </c>
+      <c r="L52" s="84"/>
       <c r="M52" s="34"/>
     </row>
+    <row r="53" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27" t="s">
+        <v>484</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>406</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="J53" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="K53" s="101"/>
+      <c r="L53" s="85"/>
+      <c r="M53" s="34"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="27"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="34"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="27"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="L28:L50"/>
+  <mergeCells count="20">
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="L28:L53"/>
     <mergeCell ref="L4:L26"/>
     <mergeCell ref="K40:K41"/>
-    <mergeCell ref="K43:K44"/>
     <mergeCell ref="K46:K47"/>
+    <mergeCell ref="K49:K50"/>
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="K34:K35"/>
     <mergeCell ref="K37:K38"/>
@@ -10095,8 +10194,14 @@
     <mergeCell ref="K25:K26"/>
     <mergeCell ref="K28:K29"/>
     <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K13:K14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>